<commit_message>
converted to enrolled change in frontend and backend
</commit_message>
<xml_diff>
--- a/Backend/excel_template/lead_template.xlsx
+++ b/Backend/excel_template/lead_template.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BLAZE GROUP\OneDrive\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45A1055-D3F3-483A-8BF9-2B9E09433A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
   </bookViews>
   <sheets>
     <sheet name="Lead Template" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>First Name</t>
   </si>
@@ -85,9 +79,6 @@
     <t>React, Node.js, TypeScript</t>
   </si>
   <si>
-    <t>United States</t>
-  </si>
-  <si>
     <t>US</t>
   </si>
   <si>
@@ -100,44 +91,14 @@
     <t>Experienced full-stack developer</t>
   </si>
   <si>
-    <t>Sarah</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>+442012345678</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>sarah.smith@example.com</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/sarahsmith</t>
-  </si>
-  <si>
-    <t>Java, Spring Boot, AWS</t>
-  </si>
-  <si>
-    <t>GB</t>
-  </si>
-  <si>
-    <t>Citizen</t>
-  </si>
-  <si>
-    <t>Indeed</t>
-  </si>
-  <si>
-    <t>Senior backend developer</t>
+    <t>United Kingdom</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -145,13 +106,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -166,8 +141,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,169 +491,130 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="15" customWidth="1"/>
-    <col min="3" max="4" width="20" customWidth="1"/>
-    <col min="5" max="6" width="30" customWidth="1"/>
-    <col min="7" max="7" width="40" customWidth="1"/>
-    <col min="8" max="8" width="30" customWidth="1"/>
-    <col min="9" max="9" width="25" customWidth="1"/>
-    <col min="10" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="40" customWidth="1"/>
+    <col min="1" max="2" width="15" style="4" customWidth="1"/>
+    <col min="3" max="4" width="20" style="4" customWidth="1"/>
+    <col min="5" max="6" width="30" style="4" customWidth="1"/>
+    <col min="7" max="7" width="40" style="4" customWidth="1"/>
+    <col min="8" max="8" width="30" style="4" customWidth="1"/>
+    <col min="9" max="9" width="25" style="4" customWidth="1"/>
+    <col min="10" max="12" width="15" style="4" customWidth="1"/>
+    <col min="13" max="13" width="40" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="M2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" t="s">
-        <v>33</v>
-      </c>
-      <c r="K3" t="s">
-        <v>34</v>
-      </c>
-      <c r="L3" t="s">
-        <v>35</v>
-      </c>
-      <c r="M3" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I2:I3" xr:uid="{1AF9F1F6-2813-4F2C-934B-E5F2ADA09A42}">
+  <dataConsolidate/>
+  <dataValidations count="5">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I2:I3">
       <formula1>"United States, Canada, United Kingdom, India, Nepal, Bangladesh, Pakistan, China, Others"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4:I9">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2">
+      <formula1>"US, CA, GB, IN, NP, BD, PK, CN,others"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K3">
+      <formula1>"H1B, L1, F1, Green Card, Citizen, H4 EAD, L2 EAD, Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L3">
+      <formula1>"Indeed,Linkedin,Referal,Other"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:M1 A3:H3 A2:H2 K2:M2 J3:M3" numberStoredAsText="1"/>
+    <ignoredError sqref="B1:M1 A2:H2 M2" numberStoredAsText="1"/>
   </ignoredErrors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EA5C6AD0-0518-4F70-A4BF-F2605B80E210}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>I4:I9</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>